<commit_message>
Otalex voc halfway done
</commit_message>
<xml_diff>
--- a/MedioAmbiente/Competency Questions.xlsx
+++ b/MedioAmbiente/Competency Questions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="72">
   <si>
     <t>Competency Question</t>
   </si>
@@ -60,12 +60,6 @@
     <t>How can I know the "Amplitud térmica Media Anual" of a region</t>
   </si>
   <si>
-    <t>What is the legend for a term in a map?</t>
-  </si>
-  <si>
-    <t>skos:legend does not exist.</t>
-  </si>
-  <si>
     <t>What is the value for a Feature in a map?</t>
   </si>
   <si>
@@ -96,12 +90,6 @@
     <t>Where is the Feature located in?</t>
   </si>
   <si>
-    <t>region and country subprop of geonames:locatedIn</t>
-  </si>
-  <si>
-    <t>What is the water consumption on a feature/region?</t>
-  </si>
-  <si>
     <t>In blue: implemented terms</t>
   </si>
   <si>
@@ -111,15 +99,9 @@
     <t>otalex:Caracteristica</t>
   </si>
   <si>
-    <t>otalex:Caracteristica, ssn:FeatureOfInterest, otalex:AmplitudTermicaAbsoluta</t>
-  </si>
-  <si>
     <t>otalex:Caracteristica, otalex:valorMinimoDeTempEnC, otalex:valorMaximoDeTempEnC</t>
   </si>
   <si>
-    <t>otalex:Caracteristica, ssn:FeatureOfInterest, otalex:AmplitudTermicaMediaAnual</t>
-  </si>
-  <si>
     <t>otalex:Caracteristica, otalex:tipoCaracteristica</t>
   </si>
   <si>
@@ -132,16 +114,124 @@
     <t>otalex:Caracteristica, geonames:countryCode</t>
   </si>
   <si>
-    <t>otalex:Caracteristica, otalex:country, otalex:region, otalex:province</t>
-  </si>
-  <si>
-    <t>otalex:Caracteristica, otalex:level1-level5</t>
-  </si>
-  <si>
-    <t>otalex:Caracteristica, otalex:consumoEnergia2001EnKwh,…, otalex:consumoEnergia2010EnKwh</t>
-  </si>
-  <si>
     <t>Will only extend locatedIn if they become URIs.</t>
+  </si>
+  <si>
+    <t>otalex:Caracteristica, otalex:codigoMunicipio, geonames:officialname, otalex:caracteristicaSituadaEnProvinciaConCodigo, otalex:característicaSituadaEnProvinciaConNombre</t>
+  </si>
+  <si>
+    <t>What is the water consumption on a feature/region in 2009?</t>
+  </si>
+  <si>
+    <t>How many rivers can we find in a particular region?</t>
+  </si>
+  <si>
+    <t>otalex:Caracteristica, otalex:numeroDeCuencasHidrograficas, geonames:name</t>
+  </si>
+  <si>
+    <t>Tipo caracteristica states the type of water body we are dealing with. Can be further refined with geolinkeddata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What are the main rivers of a region? </t>
+  </si>
+  <si>
+    <t>What is the country of a body of water?</t>
+  </si>
+  <si>
+    <t>geonames:countryCode</t>
+  </si>
+  <si>
+    <t>Under what directive has a feature been published?</t>
+  </si>
+  <si>
+    <t>otalex:RedNatura2000Aves, otalex:redNatura2000Habitats, dc:conformsTo</t>
+  </si>
+  <si>
+    <t>Where are the weather stations?</t>
+  </si>
+  <si>
+    <t>aemet:weatherStation</t>
+  </si>
+  <si>
+    <t>aemet:WeatherStation, aemet:stationName, geosparql:hasGeometry</t>
+  </si>
+  <si>
+    <t>What is the longitude and area of a Feature?</t>
+  </si>
+  <si>
+    <t>What is the ETP (evapotranspiracion) and its values?</t>
+  </si>
+  <si>
+    <t>otalex:area, otalex:longitude</t>
+  </si>
+  <si>
+    <t>otalex:superficieHectareas</t>
+  </si>
+  <si>
+    <t>What are the hectares of a Water body on the surface?</t>
+  </si>
+  <si>
+    <t>geoes:AguasSuperficiales, otalex:superficieHectareas</t>
+  </si>
+  <si>
+    <t>What are the rivers and smaller superficial bodies of whater?</t>
+  </si>
+  <si>
+    <t>geoes:Río, geoes:AguasCorrientesNaturales</t>
+  </si>
+  <si>
+    <t>otalex:CaracteristicaEvapotranspiracion, otalex:CaracteristicaETPVerano-Invierno, otalex:valorMaximo/MinimoDeETP</t>
+  </si>
+  <si>
+    <t>otalex:Caracteristica, ssn:FeatureOfInterest, otalex:CaracteristicaAmplitudTermicaAbsoluta</t>
+  </si>
+  <si>
+    <t>Cannot use SSN due to GeoKettle restrictions</t>
+  </si>
+  <si>
+    <t>otalex:Caracteristica, otalex:consumoAgua2009EnM3PorHab, otalex:CaracteristicaConsumoAgua</t>
+  </si>
+  <si>
+    <t>otalex:Caracteristica, ssn:FeatureOfInterest, otalex:CaracteristicaAmplitudTermicaMediaAnual</t>
+  </si>
+  <si>
+    <t>otalex:Caracteristica, otalex:consumoEnergia2001EnKwh,…, otalex:consumoEnergia2010EnKwh, otalex:CaracteristicaConsumoEnergia</t>
+  </si>
+  <si>
+    <t>¿Cuáles son las reservas naturales de una característica geográfica?</t>
+  </si>
+  <si>
+    <t>¿Cuáles son las vías de comunicación de una característica geográfica?</t>
+  </si>
+  <si>
+    <t>otalex:ViaDesdoblada, otalex:ViaSinDesdoblarSecundaria,  otalex:ViaSinDesdoblarPrincipal, otalex:FerrocarrilViaSimple</t>
+  </si>
+  <si>
+    <t>otalex:ReservaNatural, otalex:ParqueNatural, otalex:ParqueNacional, otalex:MonumentoNatural, otalex:PaisajeProtegido</t>
+  </si>
+  <si>
+    <t>En negro: esta por definir en la onto/por hacer label, etc. En azul: termino incorporado en la onto</t>
+  </si>
+  <si>
+    <t>¿Cuáles son las aguas superficiales de una característica?</t>
+  </si>
+  <si>
+    <t>geoes:AguasQuietas</t>
+  </si>
+  <si>
+    <t>Aguas superficiales involves embalses and albuferas. AguasQuietas is the closest parent.</t>
+  </si>
+  <si>
+    <t>What is the surface in H?</t>
+  </si>
+  <si>
+    <t>subprop of geoes:superficie</t>
+  </si>
+  <si>
+    <t>What is the ID of this Feature?</t>
+  </si>
+  <si>
+    <t>idCaracteristica</t>
   </si>
 </sst>
 </file>
@@ -166,14 +256,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="3" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="3" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -498,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -512,7 +601,7 @@
     <col min="4" max="4" width="54.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -520,10 +609,10 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="1" customFormat="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -537,131 +626,262 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="3" customFormat="1">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:5" s="2" customFormat="1">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="2" customFormat="1">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="2" customFormat="1">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="2" customFormat="1">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="2" customFormat="1">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="2" customFormat="1">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="3" customFormat="1">
-      <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="2" customFormat="1">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="2" customFormat="1">
+      <c r="A10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="3" customFormat="1">
-      <c r="A5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="D10" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="2" customFormat="1">
+      <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="3" customFormat="1">
-      <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="3" customFormat="1">
-      <c r="A7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="3" t="s">
+    </row>
+    <row r="12" spans="1:5" s="2" customFormat="1">
+      <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="3" customFormat="1">
-      <c r="A8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="B12" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="3" customFormat="1">
-      <c r="A9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
         <v>40</v>
       </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="2" t="s">
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
+      <c r="B16" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="3" customFormat="1">
+      <c r="A18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="3" customFormat="1">
+      <c r="A19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="3" customFormat="1">
+      <c r="A20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="3" customFormat="1">
+      <c r="A21" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="3" customFormat="1">
+      <c r="A22" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="3" customFormat="1">
+      <c r="A23" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="3" customFormat="1">
+      <c r="A24" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="3" customFormat="1">
+      <c r="A25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="3" customFormat="1">
+      <c r="A26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="3" customFormat="1"/>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
avances en el vocabulario de medio ambiente
</commit_message>
<xml_diff>
--- a/MedioAmbiente/Competency Questions.xlsx
+++ b/MedioAmbiente/Competency Questions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="75">
   <si>
     <t>Competency Question</t>
   </si>
@@ -232,6 +232,15 @@
   </si>
   <si>
     <t>idCaracteristica</t>
+  </si>
+  <si>
+    <t>IndiceAridad</t>
+  </si>
+  <si>
+    <t>IndiceContinentalidad</t>
+  </si>
+  <si>
+    <t>the rest follow the schema on the otalex config file. This will have to be completed from there.</t>
   </si>
 </sst>
 </file>
@@ -587,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -878,9 +887,23 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="3" customFormat="1"/>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
+    <row r="27" spans="1:4" s="3" customFormat="1">
+      <c r="B27" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="B28" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>